<commit_message>
GJES-321 - Update upload formats in Create Guest List screen.
</commit_message>
<xml_diff>
--- a/src/assets/docs/Guest List Upload format 1.xlsx
+++ b/src/assets/docs/Guest List Upload format 1.xlsx
@@ -22,10 +22,10 @@
     <t xml:space="preserve">Email </t>
   </si>
   <si>
-    <t>Note</t>
+    <t>Note/Affiliation</t>
   </si>
   <si>
-    <t>Addtional Guests</t>
+    <t>Number of addtional Guests</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 

</xml_diff>